<commit_message>
Changed the grey scheme
</commit_message>
<xml_diff>
--- a/grid81.xlsx
+++ b/grid81.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="9735" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Sheet3" sheetId="4" r:id="rId4"/>
     <sheet name="Sheet4" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet6" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="88">
   <si>
     <t>Column</t>
   </si>
@@ -281,6 +282,18 @@
   </si>
   <si>
     <t>2,3,4,5,6,7,8,9,10,11,18,19,20</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>G</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>Hex</t>
   </si>
 </sst>
 </file>
@@ -15803,8 +15816,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16049,4 +16062,330 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:J13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B3">
+        <v>128</v>
+      </c>
+      <c r="C3">
+        <v>128</v>
+      </c>
+      <c r="D3">
+        <v>128</v>
+      </c>
+      <c r="F3" t="str">
+        <f>_xlfn.BASE(B3,16)</f>
+        <v>80</v>
+      </c>
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:H3" si="0">_xlfn.BASE(C3,16)</f>
+        <v>80</v>
+      </c>
+      <c r="H3" t="str">
+        <f t="shared" si="0"/>
+        <v>80</v>
+      </c>
+      <c r="J3" t="str">
+        <f>CONCATENATE(TEXT(F3,0),TEXT(G3,0),TEXT(H3,0))</f>
+        <v>808080</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <f>B3+16</f>
+        <v>144</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:D4" si="1">C3+16</f>
+        <v>144</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="1"/>
+        <v>144</v>
+      </c>
+      <c r="F4" t="str">
+        <f t="shared" ref="F4:F11" si="2">_xlfn.BASE(B4,16)</f>
+        <v>90</v>
+      </c>
+      <c r="G4" t="str">
+        <f t="shared" ref="G4:G11" si="3">_xlfn.BASE(C4,16)</f>
+        <v>90</v>
+      </c>
+      <c r="H4" t="str">
+        <f t="shared" ref="H4:H11" si="4">_xlfn.BASE(D4,16)</f>
+        <v>90</v>
+      </c>
+      <c r="J4" t="str">
+        <f t="shared" ref="J4:J11" si="5">CONCATENATE(TEXT(F4,0),TEXT(G4,0),TEXT(H4,0))</f>
+        <v>909090</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <f t="shared" ref="B5:B14" si="6">B4+16</f>
+        <v>160</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C14" si="7">C4+16</f>
+        <v>160</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D14" si="8">D4+16</f>
+        <v>160</v>
+      </c>
+      <c r="F5" t="str">
+        <f t="shared" si="2"/>
+        <v>A0</v>
+      </c>
+      <c r="G5" t="str">
+        <f t="shared" si="3"/>
+        <v>A0</v>
+      </c>
+      <c r="H5" t="str">
+        <f t="shared" si="4"/>
+        <v>A0</v>
+      </c>
+      <c r="J5" t="str">
+        <f t="shared" si="5"/>
+        <v>A0A0A0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f t="shared" si="6"/>
+        <v>176</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="7"/>
+        <v>176</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="8"/>
+        <v>176</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="2"/>
+        <v>B0</v>
+      </c>
+      <c r="G6" t="str">
+        <f t="shared" si="3"/>
+        <v>B0</v>
+      </c>
+      <c r="H6" t="str">
+        <f t="shared" si="4"/>
+        <v>B0</v>
+      </c>
+      <c r="J6" t="str">
+        <f t="shared" si="5"/>
+        <v>B0B0B0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <f t="shared" si="6"/>
+        <v>192</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="7"/>
+        <v>192</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="8"/>
+        <v>192</v>
+      </c>
+      <c r="F7" t="str">
+        <f t="shared" si="2"/>
+        <v>C0</v>
+      </c>
+      <c r="G7" t="str">
+        <f t="shared" si="3"/>
+        <v>C0</v>
+      </c>
+      <c r="H7" t="str">
+        <f t="shared" si="4"/>
+        <v>C0</v>
+      </c>
+      <c r="J7" t="str">
+        <f t="shared" si="5"/>
+        <v>C0C0C0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <f t="shared" si="6"/>
+        <v>208</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="7"/>
+        <v>208</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="8"/>
+        <v>208</v>
+      </c>
+      <c r="F8" t="str">
+        <f t="shared" si="2"/>
+        <v>D0</v>
+      </c>
+      <c r="G8" t="str">
+        <f t="shared" si="3"/>
+        <v>D0</v>
+      </c>
+      <c r="H8" t="str">
+        <f t="shared" si="4"/>
+        <v>D0</v>
+      </c>
+      <c r="J8" t="str">
+        <f t="shared" si="5"/>
+        <v>D0D0D0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <f t="shared" si="6"/>
+        <v>224</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="7"/>
+        <v>224</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="8"/>
+        <v>224</v>
+      </c>
+      <c r="F9" t="str">
+        <f t="shared" si="2"/>
+        <v>E0</v>
+      </c>
+      <c r="G9" t="str">
+        <f t="shared" si="3"/>
+        <v>E0</v>
+      </c>
+      <c r="H9" t="str">
+        <f t="shared" si="4"/>
+        <v>E0</v>
+      </c>
+      <c r="J9" t="str">
+        <f t="shared" si="5"/>
+        <v>E0E0E0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <f t="shared" si="6"/>
+        <v>240</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="7"/>
+        <v>240</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="8"/>
+        <v>240</v>
+      </c>
+      <c r="F10" t="str">
+        <f t="shared" si="2"/>
+        <v>F0</v>
+      </c>
+      <c r="G10" t="str">
+        <f t="shared" si="3"/>
+        <v>F0</v>
+      </c>
+      <c r="H10" t="str">
+        <f t="shared" si="4"/>
+        <v>F0</v>
+      </c>
+      <c r="J10" t="str">
+        <f t="shared" si="5"/>
+        <v>F0F0F0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <f t="shared" si="6"/>
+        <v>256</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="7"/>
+        <v>256</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="8"/>
+        <v>256</v>
+      </c>
+      <c r="F11" t="str">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="G11" t="str">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+      <c r="H11" t="str">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="J11" t="str">
+        <f t="shared" si="5"/>
+        <v>100100100</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f>B11-1</f>
+        <v>255</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:D13" si="9">C11-1</f>
+        <v>255</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="9"/>
+        <v>255</v>
+      </c>
+      <c r="F13" t="str">
+        <f t="shared" ref="F13" si="10">_xlfn.BASE(B13,16)</f>
+        <v>FF</v>
+      </c>
+      <c r="G13" t="str">
+        <f t="shared" ref="G13" si="11">_xlfn.BASE(C13,16)</f>
+        <v>FF</v>
+      </c>
+      <c r="H13" t="str">
+        <f t="shared" ref="H13" si="12">_xlfn.BASE(D13,16)</f>
+        <v>FF</v>
+      </c>
+      <c r="J13" t="str">
+        <f t="shared" ref="J13" si="13">CONCATENATE(TEXT(F13,0),TEXT(G13,0),TEXT(H13,0))</f>
+        <v>FFFFFF</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>